<commit_message>
Puse en rojo lo que no hice esta semana
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Documents\Calendario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D1606A-E742-49FC-8F1D-4F4836B9F26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039EEF04-E6E9-4EFA-A6F5-F2754861C8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana1" sheetId="3" r:id="rId1"/>
@@ -624,7 +624,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -747,61 +747,55 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1322,7 +1316,7 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1363,10 +1357,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="49"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -1400,79 +1394,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52">
+      <c r="A5" s="46">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
+      <c r="A7" s="46">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1481,15 +1475,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="59" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="59" t="s">
+      <c r="F9" s="53"/>
+      <c r="G9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1498,49 +1492,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="57"/>
-      <c r="F10" s="47"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="57"/>
-      <c r="H10" s="47"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
+      <c r="A11" s="46">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="49"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1549,11 +1543,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="49"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1562,49 +1556,49 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="47"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="57"/>
-      <c r="F14" s="47"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="57"/>
-      <c r="H14" s="47"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
+      <c r="A15" s="46">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="52" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="50"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1613,15 +1607,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="46" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="59"/>
-      <c r="H17" s="46" t="s">
+      <c r="G17" s="56"/>
+      <c r="H17" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -1632,49 +1626,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="57"/>
-      <c r="F18" s="47"/>
+      <c r="F18" s="51"/>
       <c r="G18" s="57"/>
-      <c r="H18" s="47"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52">
+      <c r="A19" s="46">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="49"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1683,11 +1677,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="49"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="53"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1696,49 +1690,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
       <c r="G22" s="57"/>
-      <c r="H22" s="47"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52">
+      <c r="A23" s="46">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="58" t="s">
+      <c r="E23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="48" t="s">
+      <c r="H23" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="49"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="53"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1747,11 +1741,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="49"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1760,49 +1754,49 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="57"/>
-      <c r="F26" s="47"/>
+      <c r="F26" s="51"/>
       <c r="G26" s="57"/>
-      <c r="H26" s="47"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="52">
+      <c r="A27" s="46">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="H27" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="53"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="17"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,19 +1805,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="46" t="s">
+      <c r="F29" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="46" t="s">
+      <c r="H29" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -1834,49 +1828,49 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="47"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="51"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52">
+      <c r="A31" s="46">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="48" t="s">
+      <c r="D31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="F31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="48" t="s">
+      <c r="G31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="48" t="s">
+      <c r="H31" s="52" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="53"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="50"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1885,15 +1879,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="46" t="s">
+      <c r="E33" s="53"/>
+      <c r="F33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="49"/>
-      <c r="H33" s="46" t="s">
+      <c r="G33" s="53"/>
+      <c r="H33" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -1905,48 +1899,48 @@
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="57"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52">
+      <c r="A35" s="46">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="58" t="s">
+      <c r="D35" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="48" t="s">
+      <c r="F35" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="48" t="s">
+      <c r="G35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="48" t="s">
+      <c r="H35" s="52" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="53"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1955,11 +1949,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1969,48 +1963,48 @@
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="57"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52">
+      <c r="A39" s="46">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="58" t="s">
+      <c r="E39" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="48" t="s">
+      <c r="F39" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="48" t="s">
+      <c r="G39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="46" t="s">
+      <c r="H39" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="53"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2019,13 +2013,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="58" t="s">
+      <c r="E41" s="56"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -2038,47 +2032,47 @@
       <c r="C42" s="12"/>
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="57"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="52">
+      <c r="A43" s="46">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="58" t="s">
+      <c r="D43" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="58" t="s">
+      <c r="E43" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="48" t="s">
+      <c r="F43" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="48" t="s">
+      <c r="G43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="58" t="s">
+      <c r="H43" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="53"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="59"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2087,11 +2081,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="59"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="56"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2102,127 +2096,127 @@
       <c r="C46" s="12"/>
       <c r="D46" s="57"/>
       <c r="E46" s="57"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
       <c r="H46" s="57"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="52">
+      <c r="A47" s="46">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="58" t="s">
+      <c r="D47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="46" t="s">
+      <c r="E47" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="F47" s="48" t="s">
+      <c r="F47" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="46" t="s">
+      <c r="G47" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="58" t="s">
+      <c r="H47" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="55"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="57"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="57"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="52">
+      <c r="A49" s="46">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="58" t="s">
+      <c r="D49" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="48" t="s">
+      <c r="F49" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="46" t="s">
+      <c r="G49" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="58" t="s">
+      <c r="H49" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="55"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="57"/>
       <c r="E50" s="57"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
       <c r="H50" s="57"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="52">
+      <c r="A51" s="46">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="56" t="s">
+      <c r="E51" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="46" t="s">
+      <c r="F51" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="46" t="s">
+      <c r="G51" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H51" s="46" t="s">
+      <c r="H51" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="55"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="51"/>
       <c r="E52" s="57"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="52">
+      <c r="A53" s="46">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
@@ -2232,7 +2226,7 @@
       <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="56" t="s">
+      <c r="E53" s="59" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="16" t="s">
@@ -2247,7 +2241,7 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="55"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
@@ -2268,130 +2262,47 @@
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="52">
+      <c r="A55" s="46">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="46" t="s">
+      <c r="F55" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G55" s="46" t="s">
+      <c r="G55" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="46" t="s">
+      <c r="H55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="55"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="G35:G38"/>
     <mergeCell ref="G55:G56"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="D55:D56"/>
@@ -2416,6 +2327,89 @@
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="H51:H52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2434,8 +2428,8 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47:F48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2475,10 +2469,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="49"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -2512,79 +2506,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52">
+      <c r="A5" s="46">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
+      <c r="A7" s="46">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2593,15 +2587,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="61" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61" t="s">
+      <c r="F9" s="53"/>
+      <c r="G9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2610,49 +2604,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52">
+      <c r="A11" s="46">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="49"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2661,11 +2655,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="49"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2674,49 +2668,49 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52">
+      <c r="A15" s="46">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="60" t="s">
+      <c r="G15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="52" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="50"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2725,15 +2719,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="64" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="61"/>
-      <c r="H17" s="46" t="s">
+      <c r="G17" s="56"/>
+      <c r="H17" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -2744,49 +2738,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="47"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="52">
+      <c r="A19" s="46">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="49"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2795,11 +2789,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="49"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2808,49 +2802,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="47"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52">
+      <c r="A23" s="46">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="48" t="s">
+      <c r="H23" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="49"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="53"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2859,11 +2853,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="49"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2872,49 +2866,49 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="47"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="52">
+      <c r="A27" s="46">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="60" t="s">
+      <c r="E27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="H27" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="53"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="17"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2923,19 +2917,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="60" t="s">
+      <c r="E29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="64" t="s">
+      <c r="F29" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="46" t="s">
+      <c r="H29" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -2946,49 +2940,49 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="47"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="51"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52">
+      <c r="A31" s="46">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="60" t="s">
+      <c r="D31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="48" t="s">
+      <c r="G31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="48" t="s">
+      <c r="H31" s="52" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="53"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="50"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2997,15 +2991,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="64" t="s">
+      <c r="D33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="61"/>
-      <c r="F33" s="64" t="s">
+      <c r="E33" s="53"/>
+      <c r="F33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="49"/>
-      <c r="H33" s="46" t="s">
+      <c r="G33" s="53"/>
+      <c r="H33" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -3016,49 +3010,49 @@
         <v>3</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="52">
+      <c r="A35" s="46">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="60" t="s">
+      <c r="E35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="60" t="s">
+      <c r="F35" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="48" t="s">
+      <c r="G35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="48" t="s">
+      <c r="H35" s="52" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="53"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3067,11 +3061,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3080,49 +3074,49 @@
         <v>3</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52">
+      <c r="A39" s="46">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="64" t="s">
+      <c r="D39" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="60" t="s">
+      <c r="E39" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="60" t="s">
+      <c r="F39" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="48" t="s">
+      <c r="G39" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="46" t="s">
+      <c r="H39" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="53"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3131,13 +3125,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="60" t="s">
+      <c r="D41" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="48" t="s">
+      <c r="E41" s="56"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -3148,49 +3142,49 @@
         <v>3</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="52">
+      <c r="A43" s="46">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="60" t="s">
+      <c r="D43" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="60" t="s">
+      <c r="E43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="60" t="s">
+      <c r="F43" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="48" t="s">
+      <c r="G43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="53"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3199,11 +3193,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="56"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3212,129 +3206,129 @@
         <v>3</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="62"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="57"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="52">
+      <c r="A47" s="46">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="60" t="s">
+      <c r="D47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="64" t="s">
+      <c r="E47" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="F47" s="48" t="s">
+      <c r="F47" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="46" t="s">
+      <c r="G47" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="48" t="s">
+      <c r="H47" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="55"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="57"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="52">
+      <c r="A49" s="46">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="60" t="s">
+      <c r="D49" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="64" t="s">
+      <c r="E49" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="48" t="s">
+      <c r="F49" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="46" t="s">
+      <c r="G49" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="48" t="s">
+      <c r="H49" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="55"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="57"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="52">
+      <c r="A51" s="46">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="64" t="s">
+      <c r="E51" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="46" t="s">
+      <c r="F51" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="46" t="s">
+      <c r="G51" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H51" s="46" t="s">
+      <c r="H51" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="55"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="52">
+      <c r="A53" s="46">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
@@ -3344,7 +3338,7 @@
       <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="64" t="s">
+      <c r="E53" s="59" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="16" t="s">
@@ -3359,7 +3353,7 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="55"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
@@ -3367,7 +3361,7 @@
       <c r="D54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="62"/>
+      <c r="E54" s="57"/>
       <c r="F54" s="14" t="s">
         <v>31</v>
       </c>
@@ -3380,87 +3374,101 @@
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="52">
+      <c r="A55" s="46">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="46" t="s">
+      <c r="F55" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="G55" s="46" t="s">
+      <c r="G55" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="46" t="s">
+      <c r="H55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="55"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="107">
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="F33:F34"/>
@@ -3476,59 +3484,45 @@
     <mergeCell ref="E31:E34"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G34"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Agregue el calendario de la nueva semana
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Documents\Calendario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039EEF04-E6E9-4EFA-A6F5-F2754861C8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95EC79F-981F-431B-A968-9FE9872F2F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana1" sheetId="3" r:id="rId1"/>
     <sheet name="Semana2" sheetId="2" r:id="rId2"/>
-    <sheet name="©" sheetId="4" r:id="rId3"/>
+    <sheet name="Semana3" sheetId="5" r:id="rId3"/>
+    <sheet name="©" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Semana1!$A$1:$I$56</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="40">
   <si>
     <t>:30</t>
   </si>
@@ -147,6 +148,9 @@
   </si>
   <si>
     <t>Agenda Semana del 20 al 25</t>
+  </si>
+  <si>
+    <t>Agenda Semana del 27 al 4</t>
   </si>
 </sst>
 </file>
@@ -624,7 +628,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -747,6 +751,39 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -756,43 +793,31 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1316,7 +1341,7 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1357,10 +1382,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="56"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -1394,79 +1419,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46">
+      <c r="A5" s="57">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="G5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="55" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46">
+      <c r="A7" s="57">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1475,15 +1500,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="56" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="56" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="53"/>
+      <c r="H9" s="51"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1492,49 +1517,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="51"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46">
+      <c r="A11" s="57">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="53"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1543,11 +1568,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="53"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="51"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1556,48 +1581,48 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="51"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46">
+      <c r="A15" s="57">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="50" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="54"/>
-      <c r="E16" s="56"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="54"/>
-      <c r="G16" s="56"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
@@ -1607,15 +1632,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="58" t="s">
+      <c r="E17" s="53"/>
+      <c r="F17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="56"/>
-      <c r="H17" s="58" t="s">
+      <c r="G17" s="53"/>
+      <c r="H17" s="46" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -1626,49 +1651,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="51"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46">
+      <c r="A19" s="57">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="55" t="s">
+      <c r="G19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="50" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="53"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1677,11 +1702,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="53"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="51"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1690,49 +1715,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="51"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46">
+      <c r="A23" s="57">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="52" t="s">
+      <c r="F23" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="55" t="s">
+      <c r="G23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="50" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="48"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="53"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="51"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1741,11 +1766,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="53"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="51"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1754,40 +1779,40 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="51"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46">
+      <c r="A27" s="57">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="52" t="s">
+      <c r="E27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="52" t="s">
+      <c r="F27" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="52" t="s">
+      <c r="G27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="50" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -1805,19 +1830,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="52" t="s">
+      <c r="D29" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="52" t="s">
+      <c r="F29" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="58" t="s">
+      <c r="H29" s="46" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -1828,48 +1853,48 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="51"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="51"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="54"/>
-      <c r="H30" s="51"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="46">
+      <c r="A31" s="57">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="52" t="s">
+      <c r="F31" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="52" t="s">
+      <c r="G31" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="52" t="s">
+      <c r="H31" s="50" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="54"/>
-      <c r="E32" s="53"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="53"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
@@ -1879,15 +1904,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="59" t="s">
+      <c r="D33" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="53"/>
-      <c r="F33" s="58" t="s">
+      <c r="E33" s="51"/>
+      <c r="F33" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="53"/>
-      <c r="H33" s="58" t="s">
+      <c r="G33" s="51"/>
+      <c r="H33" s="46" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -1898,49 +1923,49 @@
         <v>3</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="46">
+      <c r="A35" s="57">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="52" t="s">
+      <c r="F35" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="52" t="s">
+      <c r="G35" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="52" t="s">
+      <c r="H35" s="50" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1949,11 +1974,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1962,49 +1987,49 @@
         <v>3</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46">
+      <c r="A39" s="57">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="55" t="s">
+      <c r="E39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="52" t="s">
+      <c r="F39" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="52" t="s">
+      <c r="G39" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="58" t="s">
+      <c r="H39" s="46" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="48"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="51"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="47"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,13 +2038,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="55" t="s">
+      <c r="E41" s="53"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -2030,49 +2055,49 @@
         <v>3</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="57"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="49"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="46">
+      <c r="A43" s="57">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="55" t="s">
+      <c r="D43" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="55" t="s">
+      <c r="E43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="52" t="s">
+      <c r="F43" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="52" t="s">
+      <c r="G43" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="56"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="53"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2081,11 +2106,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="56"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="53"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2094,129 +2119,129 @@
         <v>3</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="57"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="49"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="46">
+      <c r="A47" s="57">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="52" t="s">
+      <c r="E47" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="55" t="s">
+      <c r="G47" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="47"/>
+      <c r="A48" s="58"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="57"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="49"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="46">
+      <c r="A49" s="57">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="55" t="s">
+      <c r="D49" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="59" t="s">
+      <c r="E49" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="52" t="s">
+      <c r="F49" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="55" t="s">
+      <c r="G49" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="47"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="57"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="49"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="46">
+      <c r="A51" s="57">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="59" t="s">
+      <c r="D51" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H51" s="58" t="s">
+      <c r="F51" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="46" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="47"/>
+      <c r="A52" s="58"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="46">
+      <c r="A53" s="57">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
@@ -2226,7 +2251,7 @@
       <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="59" t="s">
+      <c r="E53" s="48" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="16" t="s">
@@ -2241,7 +2266,7 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="47"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2274,7 @@
       <c r="D54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="57"/>
+      <c r="E54" s="49"/>
       <c r="F54" s="14" t="s">
         <v>31</v>
       </c>
@@ -2262,47 +2287,130 @@
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="46">
+      <c r="A55" s="57">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="58" t="s">
+      <c r="F55" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="46" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="47"/>
+      <c r="A56" s="58"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="51"/>
+      <c r="D56" s="47"/>
       <c r="E56" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="51"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="51"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="G35:G38"/>
     <mergeCell ref="G55:G56"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="D55:D56"/>
@@ -2327,89 +2435,6 @@
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="H51:H52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2428,9 +2453,7 @@
   </sheetPr>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41:H50"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2469,10 +2492,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="56"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -2506,79 +2529,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46">
+      <c r="A5" s="57">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="G5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="55" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46">
+      <c r="A7" s="57">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
+      <c r="A8" s="59"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2587,15 +2610,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="56" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="56" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="53"/>
+      <c r="H9" s="51"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2604,49 +2627,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="51"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46">
+      <c r="A11" s="57">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="53"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2655,11 +2678,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="53"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="51"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2668,48 +2691,48 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="51"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46">
+      <c r="A15" s="57">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="50" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="54"/>
-      <c r="E16" s="56"/>
+      <c r="E16" s="53"/>
       <c r="F16" s="54"/>
-      <c r="G16" s="56"/>
+      <c r="G16" s="53"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
@@ -2719,15 +2742,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="58" t="s">
+      <c r="E17" s="53"/>
+      <c r="F17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="56"/>
-      <c r="H17" s="58" t="s">
+      <c r="G17" s="53"/>
+      <c r="H17" s="46" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -2738,49 +2761,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="51"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46">
+      <c r="A19" s="57">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="55" t="s">
+      <c r="D19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="52" t="s">
+      <c r="F19" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="50" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2789,11 +2812,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2802,49 +2825,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46">
+      <c r="A23" s="57">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="52" t="s">
+      <c r="F23" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="55" t="s">
+      <c r="G23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="50" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="48"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="51"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2853,11 +2876,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="51"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2866,40 +2889,40 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="51"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46">
+      <c r="A27" s="57">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="52" t="s">
+      <c r="E27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="52" t="s">
+      <c r="F27" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="52" t="s">
+      <c r="G27" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="52" t="s">
+      <c r="H27" s="50" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -2917,19 +2940,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="52" t="s">
+      <c r="D29" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="52" t="s">
+      <c r="F29" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="58" t="s">
+      <c r="H29" s="46" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -2940,48 +2963,48 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="51"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="51"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="54"/>
-      <c r="H30" s="51"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="46">
+      <c r="A31" s="57">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="52" t="s">
+      <c r="F31" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="52" t="s">
+      <c r="G31" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="52" t="s">
+      <c r="H31" s="50" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="54"/>
-      <c r="E32" s="53"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="53"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
@@ -2991,15 +3014,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="58" t="s">
+      <c r="D33" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="53"/>
-      <c r="F33" s="58" t="s">
+      <c r="E33" s="51"/>
+      <c r="F33" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="53"/>
-      <c r="H33" s="58" t="s">
+      <c r="G33" s="51"/>
+      <c r="H33" s="46" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -3010,49 +3033,49 @@
         <v>3</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="46">
+      <c r="A35" s="57">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="52" t="s">
+      <c r="F35" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="52" t="s">
+      <c r="G35" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="52" t="s">
+      <c r="H35" s="50" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3061,11 +3084,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3074,49 +3097,49 @@
         <v>3</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46">
+      <c r="A39" s="57">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="55" t="s">
+      <c r="E39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="52" t="s">
+      <c r="F39" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="55" t="s">
+      <c r="G39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="58" t="s">
+      <c r="H39" s="46" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="48"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="51"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="47"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3125,13 +3148,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="55" t="s">
+      <c r="E41" s="53"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -3142,49 +3165,49 @@
         <v>3</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="57"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="46">
+      <c r="A43" s="57">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="55" t="s">
+      <c r="D43" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="52" t="s">
+      <c r="F43" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="52" t="s">
+      <c r="G43" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="56"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="53"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3193,11 +3216,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="56"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="53"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3206,129 +3229,129 @@
         <v>3</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="57"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="49"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="46">
+      <c r="A47" s="57">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="52" t="s">
+      <c r="E47" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="55" t="s">
+      <c r="G47" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="47"/>
+      <c r="A48" s="58"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="57"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="49"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="46">
+      <c r="A49" s="57">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="55" t="s">
+      <c r="D49" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="59" t="s">
+      <c r="E49" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="61" t="s">
+      <c r="F49" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="55" t="s">
+      <c r="G49" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="47"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="57"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="49"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="46">
+      <c r="A51" s="57">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="59" t="s">
+      <c r="D51" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H51" s="58" t="s">
+      <c r="F51" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="46" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="47"/>
+      <c r="A52" s="58"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="46">
+      <c r="A53" s="57">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
@@ -3338,7 +3361,7 @@
       <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="59" t="s">
+      <c r="E53" s="48" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="16" t="s">
@@ -3353,7 +3376,7 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="47"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
@@ -3361,7 +3384,7 @@
       <c r="D54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="57"/>
+      <c r="E54" s="49"/>
       <c r="F54" s="14" t="s">
         <v>31</v>
       </c>
@@ -3374,48 +3397,140 @@
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="46">
+      <c r="A55" s="57">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="58" t="s">
+      <c r="F55" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="46" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="47"/>
+      <c r="A56" s="58"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="51"/>
+      <c r="D56" s="47"/>
       <c r="E56" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="51"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="51"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="107">
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="D5:D6"/>
@@ -3431,7 +3546,1085 @@
     <mergeCell ref="H7:H10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H11:H14"/>
+  </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.5" header="0.3" footer="0.25"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0">
+    <oddFooter>&amp;L&amp;8&amp;K01+048Class Schedule Template © 2017 by Vertex42.com&amp;R&amp;8&amp;K01+048https://www.vertex42.com/ExcelTemplates/class-schedule-template.html</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7327CC-5C45-4739-8DE8-8ED482915DCD}">
+  <dimension ref="A1:I56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.75" style="20" customWidth="1"/>
+    <col min="2" max="2" width="3" style="20" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="20" customWidth="1"/>
+    <col min="4" max="8" width="13.25" style="20" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="20" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="23" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="G2" s="22">
+        <v>5</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="G3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="57">
+        <v>6</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="44"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="58"/>
+      <c r="B6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="45"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="57">
+        <v>7</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="44"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="59"/>
+      <c r="B8" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="43"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="62"/>
+      <c r="I9" s="43"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
+      <c r="B10" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="45"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="45"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="57">
+        <v>8</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
+      <c r="B12" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="43"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32"/>
+      <c r="B13" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="43"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="45"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="45"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="57">
+        <v>9</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="42"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="43"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32"/>
+      <c r="B17" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="62"/>
+      <c r="F17" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="62"/>
+      <c r="H17" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="43"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="37"/>
+      <c r="B18" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="57">
+        <v>10</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
+      <c r="B20" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32"/>
+      <c r="B21" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="37"/>
+      <c r="B22" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="57">
+        <v>11</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="59"/>
+      <c r="B24" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="37"/>
+      <c r="B26" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="57">
+        <v>12</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="25"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="59"/>
+      <c r="B28" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32"/>
+      <c r="B29" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="37"/>
+      <c r="B30" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="57">
+        <v>1</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="59"/>
+      <c r="B32" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="32"/>
+      <c r="B33" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="62"/>
+      <c r="F33" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="62"/>
+      <c r="H33" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="37"/>
+      <c r="B34" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="57">
+        <v>2</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="59"/>
+      <c r="B36" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32"/>
+      <c r="B37" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="37"/>
+      <c r="B38" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="57">
+        <v>3</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="59"/>
+      <c r="B40" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="32"/>
+      <c r="B41" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
+      <c r="B42" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="57">
+        <v>4</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G43" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" s="25"/>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="59"/>
+      <c r="B44" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="32"/>
+      <c r="B45" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="37"/>
+      <c r="B46" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="57">
+        <v>5</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="58"/>
+      <c r="B48" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="57">
+        <v>6</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="58"/>
+      <c r="B50" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="57">
+        <v>7</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="58"/>
+      <c r="B52" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="63"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="57">
+        <v>8</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="H53" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="58"/>
+      <c r="B54" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" s="63"/>
+      <c r="F54" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="57">
+        <v>9</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="58"/>
+      <c r="B56" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="63"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="107">
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H19:H22"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E18"/>
@@ -3446,95 +4639,28 @@
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.5" header="0.3" footer="0.25"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0">
-    <oddFooter>&amp;L&amp;8&amp;K01+048Class Schedule Template © 2017 by Vertex42.com&amp;R&amp;8&amp;K01+048https://www.vertex42.com/ExcelTemplates/class-schedule-template.html</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>

</xml_diff>

<commit_message>
Puse en rojo lo que no hice en la semana
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Documents\Calendario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95EC79F-981F-431B-A968-9FE9872F2F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23748C8F-6B36-4DE5-8F2B-3D852D05314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,7 +628,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -751,76 +751,49 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1382,10 +1355,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="49"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -1419,79 +1392,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57">
+      <c r="A5" s="46">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57">
+      <c r="A7" s="46">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1500,15 +1473,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="53" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="53" t="s">
+      <c r="F9" s="53"/>
+      <c r="G9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="51"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,49 +1490,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57">
+      <c r="A11" s="46">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="51"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1568,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="51"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1581,48 +1554,48 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57">
+      <c r="A15" s="46">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="50" t="s">
+      <c r="H15" s="52" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="54"/>
-      <c r="E16" s="53"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="54"/>
-      <c r="G16" s="53"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
@@ -1632,15 +1605,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="46" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="46" t="s">
+      <c r="G17" s="56"/>
+      <c r="H17" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -1651,49 +1624,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="47"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57">
+      <c r="A19" s="46">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="51"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,11 +1675,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="51"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="53"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1715,49 +1688,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="47"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="57">
+      <c r="A23" s="46">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="50" t="s">
+      <c r="H23" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="59"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="51"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="53"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1766,11 +1739,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="51"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1779,40 +1752,40 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="47"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="57">
+      <c r="A27" s="46">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="50" t="s">
+      <c r="D27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="50" t="s">
+      <c r="F27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="50" t="s">
+      <c r="H27" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -1830,19 +1803,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="50" t="s">
+      <c r="D29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="50" t="s">
+      <c r="F29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="46" t="s">
+      <c r="H29" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -1853,48 +1826,48 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="47"/>
+      <c r="F30" s="51"/>
       <c r="G30" s="54"/>
-      <c r="H30" s="47"/>
+      <c r="H30" s="51"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="57">
+      <c r="A31" s="46">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="50" t="s">
+      <c r="D31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="50" t="s">
+      <c r="F31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="50" t="s">
+      <c r="H31" s="52" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="54"/>
-      <c r="E32" s="51"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="51"/>
+      <c r="G32" s="53"/>
       <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
@@ -1904,15 +1877,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="51"/>
-      <c r="F33" s="46" t="s">
+      <c r="E33" s="53"/>
+      <c r="F33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="51"/>
-      <c r="H33" s="46" t="s">
+      <c r="G33" s="53"/>
+      <c r="H33" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -1923,49 +1896,49 @@
         <v>3</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57">
+      <c r="A35" s="46">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="50" t="s">
+      <c r="F35" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="50" t="s">
+      <c r="G35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="50" t="s">
+      <c r="H35" s="52" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1974,11 +1947,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1987,49 +1960,49 @@
         <v>3</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="57">
+      <c r="A39" s="46">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="50" t="s">
+      <c r="F39" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="50" t="s">
+      <c r="G39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="46" t="s">
+      <c r="H39" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2038,13 +2011,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="52" t="s">
+      <c r="D41" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="53"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="52" t="s">
+      <c r="E41" s="56"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -2055,49 +2028,49 @@
         <v>3</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="49"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="57"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="57">
+      <c r="A43" s="46">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="52" t="s">
+      <c r="D43" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="50" t="s">
+      <c r="F43" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="50" t="s">
+      <c r="G43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="52" t="s">
+      <c r="H43" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="53"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2106,11 +2079,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="53"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="56"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2119,129 +2092,129 @@
         <v>3</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="49"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="57"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="57">
+      <c r="A47" s="46">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="52" t="s">
+      <c r="D47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="50" t="s">
+      <c r="E47" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="52" t="s">
+      <c r="G47" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="58"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="49"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="57"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="57">
+      <c r="A49" s="46">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="52" t="s">
+      <c r="D49" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="48" t="s">
+      <c r="E49" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="50" t="s">
+      <c r="F49" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="52" t="s">
+      <c r="G49" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="58"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="49"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="57"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="57">
+      <c r="A51" s="46">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="48" t="s">
+      <c r="D51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H51" s="46" t="s">
+      <c r="F51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="58"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="57">
+      <c r="A53" s="46">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
@@ -2251,7 +2224,7 @@
       <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="48" t="s">
+      <c r="E53" s="59" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="16" t="s">
@@ -2266,7 +2239,7 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
@@ -2274,7 +2247,7 @@
       <c r="D54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="49"/>
+      <c r="E54" s="57"/>
       <c r="F54" s="14" t="s">
         <v>31</v>
       </c>
@@ -2287,130 +2260,47 @@
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="57">
+      <c r="A55" s="46">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="46" t="s">
+      <c r="F55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="58"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="G35:G38"/>
     <mergeCell ref="G55:G56"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="D55:D56"/>
@@ -2435,6 +2325,89 @@
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="H51:H52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A43:A44"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2492,10 +2465,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="49"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -2529,79 +2502,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57">
+      <c r="A5" s="46">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57">
+      <c r="A7" s="46">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2610,15 +2583,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="53" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="53" t="s">
+      <c r="F9" s="53"/>
+      <c r="G9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="51"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2627,49 +2600,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57">
+      <c r="A11" s="46">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="51"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2678,11 +2651,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="51"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2691,48 +2664,48 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57">
+      <c r="A15" s="46">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="50" t="s">
+      <c r="H15" s="52" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="54"/>
-      <c r="E16" s="53"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="54"/>
-      <c r="G16" s="53"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
@@ -2742,15 +2715,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="46" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="46" t="s">
+      <c r="G17" s="56"/>
+      <c r="H17" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -2761,49 +2734,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="47"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57">
+      <c r="A19" s="46">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="50" t="s">
+      <c r="F19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="50" t="s">
+      <c r="G19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2812,11 +2785,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2825,49 +2798,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="57">
+      <c r="A23" s="46">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="50" t="s">
+      <c r="H23" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="59"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="51"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="53"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2876,11 +2849,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="51"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2889,40 +2862,40 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="47"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="57">
+      <c r="A27" s="46">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="50" t="s">
+      <c r="F27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="50" t="s">
+      <c r="H27" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
@@ -2940,19 +2913,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="50" t="s">
+      <c r="D29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="50" t="s">
+      <c r="F29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="46" t="s">
+      <c r="H29" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -2963,48 +2936,48 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="54"/>
-      <c r="F30" s="47"/>
+      <c r="F30" s="51"/>
       <c r="G30" s="54"/>
-      <c r="H30" s="47"/>
+      <c r="H30" s="51"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="57">
+      <c r="A31" s="46">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="50" t="s">
+      <c r="D31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="50" t="s">
+      <c r="F31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="50" t="s">
+      <c r="H31" s="52" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="54"/>
-      <c r="E32" s="51"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="54"/>
-      <c r="G32" s="51"/>
+      <c r="G32" s="53"/>
       <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
@@ -3014,15 +2987,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="51"/>
-      <c r="F33" s="46" t="s">
+      <c r="E33" s="53"/>
+      <c r="F33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="51"/>
-      <c r="H33" s="46" t="s">
+      <c r="G33" s="53"/>
+      <c r="H33" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -3033,49 +3006,49 @@
         <v>3</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57">
+      <c r="A35" s="46">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="50" t="s">
+      <c r="D35" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="50" t="s">
+      <c r="F35" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="50" t="s">
+      <c r="G35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="50" t="s">
+      <c r="H35" s="52" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3084,11 +3057,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3097,49 +3070,49 @@
         <v>3</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="57">
+      <c r="A39" s="46">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="52" t="s">
+      <c r="E39" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="50" t="s">
+      <c r="F39" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="52" t="s">
+      <c r="G39" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="46" t="s">
+      <c r="H39" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3148,13 +3121,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="52" t="s">
+      <c r="D41" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="53"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="52" t="s">
+      <c r="E41" s="56"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -3165,49 +3138,49 @@
         <v>3</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
       <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="57">
+      <c r="A43" s="46">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="52" t="s">
+      <c r="D43" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="50" t="s">
+      <c r="F43" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="50" t="s">
+      <c r="G43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="52" t="s">
+      <c r="H43" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="53"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3216,11 +3189,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="53"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="56"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -3229,129 +3202,129 @@
         <v>3</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="49"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="57"/>
       <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="57">
+      <c r="A47" s="46">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="52" t="s">
+      <c r="D47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="50" t="s">
+      <c r="E47" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="52" t="s">
+      <c r="G47" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="58"/>
+      <c r="A48" s="47"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="49"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="57"/>
       <c r="I48" s="13"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="57">
+      <c r="A49" s="46">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="52" t="s">
+      <c r="D49" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="48" t="s">
+      <c r="E49" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="50" t="s">
+      <c r="F49" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="52" t="s">
+      <c r="G49" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="58"/>
+      <c r="A50" s="47"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="49"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="57"/>
       <c r="I50" s="13"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="57">
+      <c r="A51" s="46">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="48" t="s">
+      <c r="D51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H51" s="46" t="s">
+      <c r="F51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="58"/>
+      <c r="A52" s="47"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
       <c r="I52" s="13"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="57">
+      <c r="A53" s="46">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
@@ -3361,7 +3334,7 @@
       <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="48" t="s">
+      <c r="E53" s="59" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="16" t="s">
@@ -3376,7 +3349,7 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
+      <c r="A54" s="47"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
@@ -3384,7 +3357,7 @@
       <c r="D54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E54" s="49"/>
+      <c r="E54" s="57"/>
       <c r="F54" s="14" t="s">
         <v>31</v>
       </c>
@@ -3397,87 +3370,101 @@
       <c r="I54" s="13"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="57">
+      <c r="A55" s="46">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="46" t="s">
+      <c r="F55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="58"/>
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="51"/>
       <c r="E56" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="107">
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="F33:F34"/>
@@ -3493,59 +3480,45 @@
     <mergeCell ref="E31:E34"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G34"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G18"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3562,10 +3535,10 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.75" style="20" customWidth="1"/>
     <col min="2" max="2" width="3" style="20" customWidth="1"/>
@@ -3602,10 +3575,10 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="49"/>
       <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
@@ -3639,79 +3612,79 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57">
+      <c r="A5" s="46">
         <v>6</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="44"/>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="50" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="45"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57">
+      <c r="A7" s="46">
         <v>7</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="42"/>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="E7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="61" t="s">
+      <c r="G7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="H7" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="43"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3720,15 +3693,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62" t="s">
+      <c r="D9" s="53"/>
+      <c r="E9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62" t="s">
+      <c r="F9" s="53"/>
+      <c r="G9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="62"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3737,49 +3710,49 @@
         <v>3</v>
       </c>
       <c r="C10" s="45"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57">
+      <c r="A11" s="46">
         <v>8</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="42"/>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="61" t="s">
+      <c r="G11" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3788,11 +3761,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="43"/>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3801,49 +3774,49 @@
         <v>3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="51"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57">
+      <c r="A15" s="46">
         <v>9</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="18"/>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="61" t="s">
+      <c r="H15" s="52" t="s">
         <v>28</v>
       </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="64"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="54"/>
       <c r="I16" s="43"/>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3852,15 +3825,15 @@
         <v>0</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="65" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="65" t="s">
+      <c r="G17" s="56"/>
+      <c r="H17" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="43"/>
@@ -3871,49 +3844,49 @@
         <v>3</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57">
+      <c r="A19" s="46">
         <v>10</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="18"/>
-      <c r="D19" s="61" t="s">
+      <c r="D19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="61" t="s">
+      <c r="F19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="61" t="s">
+      <c r="G19" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3922,11 +3895,11 @@
         <v>0</v>
       </c>
       <c r="C21" s="18"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3935,49 +3908,49 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="57">
+      <c r="A23" s="46">
         <v>11</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="61" t="s">
+      <c r="G23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="61" t="s">
+      <c r="H23" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="59"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
       <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3986,11 +3959,11 @@
         <v>0</v>
       </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -3999,49 +3972,49 @@
         <v>3</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="57">
+      <c r="A27" s="46">
         <v>12</v>
       </c>
       <c r="B27" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="61" t="s">
+      <c r="E27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="61" t="s">
+      <c r="F27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="61" t="s">
+      <c r="G27" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="61" t="s">
+      <c r="H27" s="52" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="59"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="17"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4050,19 +4023,19 @@
         <v>0</v>
       </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="61" t="s">
+      <c r="D29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="61" t="s">
+      <c r="F29" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="65" t="s">
+      <c r="H29" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="18"/>
@@ -4073,49 +4046,49 @@
         <v>3</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="63"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="51"/>
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="57">
+      <c r="A31" s="46">
         <v>1</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="61" t="s">
+      <c r="D31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="61" t="s">
+      <c r="E31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="61" t="s">
+      <c r="F31" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="61" t="s">
+      <c r="G31" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="61" t="s">
+      <c r="H31" s="52" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="59"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="17"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="64"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="54"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4124,15 +4097,15 @@
         <v>0</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="65" t="s">
+      <c r="D33" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="62"/>
-      <c r="F33" s="65" t="s">
+      <c r="E33" s="53"/>
+      <c r="F33" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="62"/>
-      <c r="H33" s="65" t="s">
+      <c r="G33" s="53"/>
+      <c r="H33" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="18"/>
@@ -4143,49 +4116,49 @@
         <v>3</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="57">
+      <c r="A35" s="46">
         <v>2</v>
       </c>
       <c r="B35" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="61" t="s">
+      <c r="D35" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="61" t="s">
+      <c r="F35" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="61" t="s">
+      <c r="G35" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="61" t="s">
+      <c r="H35" s="52" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="59"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="17"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4194,11 +4167,11 @@
         <v>0</v>
       </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4207,49 +4180,49 @@
         <v>3</v>
       </c>
       <c r="C38" s="12"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="57">
+      <c r="A39" s="46">
         <v>3</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="18"/>
-      <c r="D39" s="65" t="s">
+      <c r="D39" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="61" t="s">
+      <c r="E39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="61" t="s">
+      <c r="F39" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="61" t="s">
+      <c r="G39" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="65" t="s">
+      <c r="H39" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C40" s="17"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="62"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="63"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="51"/>
       <c r="I40" s="17"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4258,13 +4231,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="18"/>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="61" t="s">
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="18"/>
@@ -4275,49 +4248,49 @@
         <v>3</v>
       </c>
       <c r="C42" s="12"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="57">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="46">
         <v>4</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="18"/>
-      <c r="D43" s="61" t="s">
+      <c r="D43" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="61" t="s">
+      <c r="E43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="61" t="s">
+      <c r="F43" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="61" t="s">
+      <c r="G43" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="61" t="s">
+      <c r="H43" s="52" t="s">
         <v>33</v>
       </c>
       <c r="I43" s="25"/>
     </row>
-    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="59"/>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
       <c r="B44" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="17"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
       <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4326,11 +4299,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="18"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4339,286 +4312,236 @@
         <v>3</v>
       </c>
       <c r="C46" s="12"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="57">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="46">
         <v>5</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="15"/>
-      <c r="D47" s="61" t="s">
+      <c r="D47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="61" t="s">
+      <c r="E47" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="61" t="s">
+      <c r="G47" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I47" s="15"/>
     </row>
-    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="58"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="47"/>
       <c r="B48" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="57"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="57">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="46">
         <v>6</v>
       </c>
       <c r="B49" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="15"/>
-      <c r="D49" s="61" t="s">
+      <c r="D49" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="65" t="s">
+      <c r="E49" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="61" t="s">
+      <c r="F49" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="61" t="s">
+      <c r="G49" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="55" t="s">
         <v>33</v>
       </c>
       <c r="I49" s="15"/>
     </row>
-    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="58"/>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="47"/>
       <c r="B50" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="13"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="63"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="57"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="57">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="46">
         <v>7</v>
       </c>
       <c r="B51" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="15"/>
-      <c r="D51" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" s="65" t="s">
+      <c r="D51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="G51" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H51" s="65" t="s">
+      <c r="F51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="58"/>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="47"/>
       <c r="B52" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="63"/>
-      <c r="H52" s="63"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="57">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="46">
         <v>8</v>
       </c>
       <c r="B53" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="15"/>
-      <c r="D53" s="66" t="s">
+      <c r="D53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E53" s="65" t="s">
+      <c r="E53" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="F53" s="66" t="s">
+      <c r="F53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G53" s="66" t="s">
+      <c r="G53" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H53" s="66" t="s">
+      <c r="H53" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I53" s="15"/>
     </row>
-    <row r="54" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="47"/>
       <c r="B54" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="13"/>
-      <c r="D54" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" s="63"/>
-      <c r="F54" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="G54" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="H54" s="67" t="s">
+      <c r="D54" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54" s="51"/>
+      <c r="F54" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="14" t="s">
         <v>31</v>
       </c>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="57">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="46">
         <v>9</v>
       </c>
       <c r="B55" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="15"/>
-      <c r="D55" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="E55" s="68" t="s">
+      <c r="D55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F55" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="65" t="s">
+      <c r="F55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="58" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="15"/>
     </row>
-    <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="58"/>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="47"/>
       <c r="B56" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="F56" s="63"/>
-      <c r="G56" s="63"/>
-      <c r="H56" s="63"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
       <c r="I56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="F43:F46"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="F23:F26"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="D19:D22"/>
     <mergeCell ref="E19:E22"/>
@@ -4634,27 +4557,77 @@
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="H17:H18"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>